<commit_message>
Clean up Beta_calc.R code
</commit_message>
<xml_diff>
--- a/final_betas.xlsx
+++ b/final_betas.xlsx
@@ -421,16 +421,16 @@
         </is>
       </c>
       <c r="E2">
-        <v>0.9999995175812678</v>
+        <v>1.000000102806806</v>
       </c>
       <c r="F2">
-        <v>2.671344049807348E-07</v>
+        <v>2.949214424937967E-07</v>
       </c>
       <c r="G2">
-        <v>3743432.141035468</v>
+        <v>3390733.797959907</v>
       </c>
       <c r="H2">
-        <v>2.193457655352071E-148</v>
+        <v>2.603370599182205E-147</v>
       </c>
     </row>
     <row r="3">
@@ -455,16 +455,16 @@
         </is>
       </c>
       <c r="E3">
-        <v>1.234338337303423</v>
+        <v>1.23433784887034</v>
       </c>
       <c r="F3">
-        <v>0.3166090217452364</v>
+        <v>0.3166090886962632</v>
       </c>
       <c r="G3">
-        <v>3.898620230400919</v>
+        <v>3.898617863287222</v>
       </c>
       <c r="H3">
-        <v>0.0006425064928510495</v>
+        <v>0.0006425103851562793</v>
       </c>
     </row>
     <row r="4">
@@ -489,16 +489,16 @@
         </is>
       </c>
       <c r="E4">
-        <v>1.232534205684902</v>
+        <v>1.232533273701805</v>
       </c>
       <c r="F4">
-        <v>0.4287927740397365</v>
+        <v>0.4287928708670447</v>
       </c>
       <c r="G4">
-        <v>2.874428582536426</v>
+        <v>2.874425759946871</v>
       </c>
       <c r="H4">
-        <v>0.008147235493885093</v>
+        <v>0.008147289954327742</v>
       </c>
     </row>
     <row r="5">
@@ -523,16 +523,16 @@
         </is>
       </c>
       <c r="E5">
-        <v>1.371350309352195</v>
+        <v>1.371350092038687</v>
       </c>
       <c r="F5">
-        <v>0.4245477500224174</v>
+        <v>0.424547767205771</v>
       </c>
       <c r="G5">
-        <v>3.230143863157404</v>
+        <v>3.230143220548413</v>
       </c>
       <c r="H5">
-        <v>0.003451015695728496</v>
+        <v>0.003451021144898397</v>
       </c>
     </row>
     <row r="6">
@@ -557,16 +557,16 @@
         </is>
       </c>
       <c r="E6">
-        <v>1.038715875682156</v>
+        <v>1.038715776342111</v>
       </c>
       <c r="F6">
-        <v>0.3312664526359915</v>
+        <v>0.3312664567389792</v>
       </c>
       <c r="G6">
-        <v>3.135590300245516</v>
+        <v>3.135589961529262</v>
       </c>
       <c r="H6">
-        <v>0.004349320177609629</v>
+        <v>0.004349323766392233</v>
       </c>
     </row>
     <row r="7">
@@ -591,16 +591,16 @@
         </is>
       </c>
       <c r="E7">
-        <v>1.499985265206973</v>
+        <v>1.499984864011523</v>
       </c>
       <c r="F7">
-        <v>0.3309359894835456</v>
+        <v>0.3309360513054669</v>
       </c>
       <c r="G7">
-        <v>4.532554067473382</v>
+        <v>4.532552008445217</v>
       </c>
       <c r="H7">
-        <v>0.0001251688762539333</v>
+        <v>0.0001251695443991448</v>
       </c>
     </row>
     <row r="8">
@@ -625,16 +625,16 @@
         </is>
       </c>
       <c r="E8">
-        <v>1.432970073639622</v>
+        <v>1.432969991410402</v>
       </c>
       <c r="F8">
-        <v>0.5636909581156268</v>
+        <v>0.5636909536328849</v>
       </c>
       <c r="G8">
-        <v>2.542120026955771</v>
+        <v>2.542119901295512</v>
       </c>
       <c r="H8">
-        <v>0.01759203495479226</v>
+        <v>0.01759203995199525</v>
       </c>
     </row>
     <row r="9">
@@ -659,16 +659,16 @@
         </is>
       </c>
       <c r="E9">
-        <v>1.261902334960643</v>
+        <v>1.261901771453531</v>
       </c>
       <c r="F9">
-        <v>0.2571947601229166</v>
+        <v>0.2571949016513472</v>
       </c>
       <c r="G9">
-        <v>4.90640763582261</v>
+        <v>4.906402744966393</v>
       </c>
       <c r="H9">
-        <v>4.748890557340036E-05</v>
+        <v>4.748950712240083E-05</v>
       </c>
     </row>
     <row r="10">
@@ -693,16 +693,16 @@
         </is>
       </c>
       <c r="E10">
-        <v>0.8905376142288768</v>
+        <v>0.8905381796509941</v>
       </c>
       <c r="F10">
-        <v>0.2076664589623528</v>
+        <v>0.2076663778679619</v>
       </c>
       <c r="G10">
-        <v>4.288307407361915</v>
+        <v>4.288311804702515</v>
       </c>
       <c r="H10">
-        <v>0.0002356153847776379</v>
+        <v>0.0002356127056390428</v>
       </c>
     </row>
     <row r="11">
@@ -727,16 +727,16 @@
         </is>
       </c>
       <c r="E11">
-        <v>0.6464835833566334</v>
+        <v>0.6464830737655988</v>
       </c>
       <c r="F11">
-        <v>0.2964192120140854</v>
+        <v>0.296419247169613</v>
       </c>
       <c r="G11">
-        <v>2.180977335996404</v>
+        <v>2.180975358174623</v>
       </c>
       <c r="H11">
-        <v>0.03880252868347944</v>
+        <v>0.03880269101825961</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Sp500 betas, add more code checks, add MTCH to portfolio.
</commit_message>
<xml_diff>
--- a/final_betas.xlsx
+++ b/final_betas.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,20 +417,20 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2022-06-27 - 2024-09-23</t>
+          <t>2022-10-03 - 2024-09-20</t>
         </is>
       </c>
       <c r="E2">
-        <v>0.9999995855707912</v>
+        <v>1.004615391668081</v>
       </c>
       <c r="F2">
-        <v>3.628399878519052E-07</v>
+        <v>0.00995854079907098</v>
       </c>
       <c r="G2">
-        <v>2756034.668314854</v>
+        <v>100.8797786681559</v>
       </c>
       <c r="H2">
-        <v>4.63192447538027E-145</v>
+        <v>1.07173329996564E-29</v>
       </c>
     </row>
     <row r="3">
@@ -451,20 +451,20 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2022-06-27 - 2024-09-23</t>
+          <t>2022-10-03 - 2024-09-20</t>
         </is>
       </c>
       <c r="E3">
-        <v>1.234336982918261</v>
+        <v>1.310756136243378</v>
       </c>
       <c r="F3">
-        <v>0.316609168455486</v>
+        <v>0.3588983204424652</v>
       </c>
       <c r="G3">
-        <v>3.898614146077088</v>
+        <v>3.652165701492895</v>
       </c>
       <c r="H3">
-        <v>0.0006425164975062915</v>
+        <v>0.001487785739533245</v>
       </c>
     </row>
     <row r="4">
@@ -485,20 +485,20 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2022-06-27 - 2024-09-23</t>
+          <t>2022-10-03 - 2024-09-20</t>
         </is>
       </c>
       <c r="E4">
-        <v>1.232532250504969</v>
+        <v>1.445110674142892</v>
       </c>
       <c r="F4">
-        <v>0.4287929265616104</v>
+        <v>0.5814516207294718</v>
       </c>
       <c r="G4">
-        <v>2.874423000370726</v>
+        <v>2.485349808346736</v>
       </c>
       <c r="H4">
-        <v>0.008147343199292324</v>
+        <v>0.02144572449122563</v>
       </c>
     </row>
     <row r="5">
@@ -519,20 +519,20 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2022-06-27 - 2024-09-23</t>
+          <t>2022-10-03 - 2024-09-20</t>
         </is>
       </c>
       <c r="E5">
-        <v>1.371349996585742</v>
+        <v>2.150786540329463</v>
       </c>
       <c r="F5">
-        <v>0.4245477141983463</v>
+        <v>0.4930045616409439</v>
       </c>
       <c r="G5">
-        <v>3.230143399017466</v>
+        <v>4.362609816774647</v>
       </c>
       <c r="H5">
-        <v>0.00345101963152286</v>
+        <v>0.0002730074041201833</v>
       </c>
     </row>
     <row r="6">
@@ -553,20 +553,20 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2022-06-27 - 2024-09-23</t>
+          <t>2022-10-03 - 2024-09-20</t>
         </is>
       </c>
       <c r="E6">
-        <v>1.03871568531502</v>
+        <v>1.244794109883067</v>
       </c>
       <c r="F6">
-        <v>0.3312664180380399</v>
+        <v>0.4502407874277962</v>
       </c>
       <c r="G6">
-        <v>3.135590053066418</v>
+        <v>2.764729772694553</v>
       </c>
       <c r="H6">
-        <v>0.004349322796533106</v>
+        <v>0.01161085469338004</v>
       </c>
     </row>
     <row r="7">
@@ -587,20 +587,20 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2022-06-27 - 2024-09-23</t>
+          <t>2022-10-03 - 2024-09-20</t>
         </is>
       </c>
       <c r="E7">
-        <v>1.499983840739705</v>
+        <v>1.808481337309522</v>
       </c>
       <c r="F7">
-        <v>0.3309361713610704</v>
+        <v>0.4536861211055292</v>
       </c>
       <c r="G7">
-        <v>4.532547272093556</v>
+        <v>3.986194977493839</v>
       </c>
       <c r="H7">
-        <v>0.0001251710813370835</v>
+        <v>0.0006714998236065933</v>
       </c>
     </row>
     <row r="8">
@@ -621,20 +621,20 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2022-06-27 - 2024-09-23</t>
+          <t>2022-10-03 - 2024-09-20</t>
         </is>
       </c>
       <c r="E8">
-        <v>1.43296950148672</v>
+        <v>1.820325349745084</v>
       </c>
       <c r="F8">
-        <v>0.5636909264188159</v>
+        <v>0.8016265339072233</v>
       </c>
       <c r="G8">
-        <v>2.542119154889572</v>
+        <v>2.270789791441409</v>
       </c>
       <c r="H8">
-        <v>0.01759206963477195</v>
+        <v>0.03380331770559451</v>
       </c>
     </row>
     <row r="9">
@@ -655,20 +655,20 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2022-06-27 - 2024-09-23</t>
+          <t>2022-10-03 - 2024-09-20</t>
         </is>
       </c>
       <c r="E9">
-        <v>1.261900644358862</v>
+        <v>1.394180262023718</v>
       </c>
       <c r="F9">
-        <v>0.2571949609079614</v>
+        <v>0.3565260215679585</v>
       </c>
       <c r="G9">
-        <v>4.906397232294297</v>
+        <v>3.910458641678611</v>
       </c>
       <c r="H9">
-        <v>4.749018516057728E-05</v>
+        <v>0.0008045976145165426</v>
       </c>
     </row>
     <row r="10">
@@ -689,20 +689,20 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2022-06-27 - 2024-09-23</t>
+          <t>2022-10-03 - 2024-09-20</t>
         </is>
       </c>
       <c r="E10">
-        <v>0.8905383975732132</v>
+        <v>1.110218960991679</v>
       </c>
       <c r="F10">
-        <v>0.2076664067284261</v>
+        <v>0.2922566511359825</v>
       </c>
       <c r="G10">
-        <v>4.288312258119855</v>
+        <v>3.798780820475191</v>
       </c>
       <c r="H10">
-        <v>0.0002356124293901829</v>
+        <v>0.00105002869816451</v>
       </c>
     </row>
     <row r="11">
@@ -723,20 +723,54 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2022-06-27 - 2024-09-23</t>
+          <t>2022-10-03 - 2024-09-20</t>
         </is>
       </c>
       <c r="E11">
-        <v>0.6464829404525255</v>
+        <v>0.8432122289204602</v>
       </c>
       <c r="F11">
-        <v>0.2964191845093321</v>
+        <v>0.4147805513157619</v>
       </c>
       <c r="G11">
-        <v>2.180975369467601</v>
+        <v>2.032911683649661</v>
       </c>
       <c r="H11">
-        <v>0.03880269009135782</v>
+        <v>0.05489635629588587</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Tinder</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MTCH</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Market Returns</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>2022-10-03 - 2024-09-20</t>
+        </is>
+      </c>
+      <c r="E12">
+        <v>2.292724702980512</v>
+      </c>
+      <c r="F12">
+        <v>0.5988664939774522</v>
+      </c>
+      <c r="G12">
+        <v>3.828440438791413</v>
+      </c>
+      <c r="H12">
+        <v>0.0009784048750956023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>